<commit_message>
Updated Code base with Edit Blog and Incomplete Multiple Browser Executions
</commit_message>
<xml_diff>
--- a/TestData/BlogTestData/blogTestCase.xlsx
+++ b/TestData/BlogTestData/blogTestCase.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\POM_for_Bottle\WebApp\TestData\BlogTestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E572A4EC-B476-4DA1-B4E1-5158BFC9FFB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E515228-A019-4E37-AD89-4FA2FE8529B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="new_blog" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="46">
   <si>
     <t>username</t>
   </si>
@@ -60,12 +61,6 @@
     <t>imgPath</t>
   </si>
   <si>
-    <t xml:space="preserve">This is short Description </t>
-  </si>
-  <si>
-    <t>test_auto_dateSheet</t>
-  </si>
-  <si>
     <t>E:\POM_for_Bottle\WebApp\TestData\BlogTestData\SampleImage\sampel_leather_1.jpg</t>
   </si>
   <si>
@@ -93,21 +88,6 @@
     <t>This is example of Order list - 1,This is example of Order list - 6</t>
   </si>
   <si>
-    <t>Automation Test Blog -1</t>
-  </si>
-  <si>
-    <t>Automation Test Blog -2</t>
-  </si>
-  <si>
-    <t>Automation Test Blog -3</t>
-  </si>
-  <si>
-    <t>Automation Test Blog -4</t>
-  </si>
-  <si>
-    <t>Automation Test Blog -5</t>
-  </si>
-  <si>
     <t>imgBlogLayout</t>
   </si>
   <si>
@@ -139,6 +119,51 @@
   </si>
   <si>
     <t>E:\POM_for_Bottle\WebApp\TestData\BlogTestData\SampleImage\sampel_leather_1.jpg, E:\POM_for_Bottle\WebApp\TestData\BlogTestData\SampleImage\sampel_leather_2.jpg, E:\POM_for_Bottle\WebApp\TestData\BlogTestData\SampleImage\sampel_leather_3.jpg, E:\POM_for_Bottle\WebApp\TestData\BlogTestData\SampleImage\sampel_leather_4.jpg, E:\POM_for_Bottle\WebApp\TestData\BlogTestData\SampleImage\sampel_leather_5.jpg</t>
+  </si>
+  <si>
+    <t>This is short Description 17</t>
+  </si>
+  <si>
+    <t>This is short Description 18</t>
+  </si>
+  <si>
+    <t>This is short Description 19</t>
+  </si>
+  <si>
+    <t>This is short Description 20</t>
+  </si>
+  <si>
+    <t>test_auto_dateSheet-17</t>
+  </si>
+  <si>
+    <t>test_auto_dateSheet-18</t>
+  </si>
+  <si>
+    <t>test_auto_dateSheet-19</t>
+  </si>
+  <si>
+    <t>test_auto_dateSheet-20</t>
+  </si>
+  <si>
+    <t>Automation Test Blog -17</t>
+  </si>
+  <si>
+    <t>Automation Test Blog -18</t>
+  </si>
+  <si>
+    <t>Automation Test Blog -19</t>
+  </si>
+  <si>
+    <t>Automation Test Blog -20</t>
+  </si>
+  <si>
+    <t>This is short Description 21</t>
+  </si>
+  <si>
+    <t>Automation Test Blog -21</t>
+  </si>
+  <si>
+    <t>test_auto_dateSheet-21</t>
   </si>
 </sst>
 </file>
@@ -473,14 +498,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N6"/>
+  <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J14" activeCellId="1" sqref="L3:L6 J14"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="3" max="3" width="23" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10.5546875" customWidth="1"/>
     <col min="8" max="8" width="12.33203125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="15.33203125" customWidth="1"/>
@@ -507,10 +533,10 @@
         <v>7</v>
       </c>
       <c r="G1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="H1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="I1" t="s">
         <v>9</v>
@@ -519,16 +545,16 @@
         <v>10</v>
       </c>
       <c r="K1" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="L1" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="M1" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="N1" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.3">
@@ -539,204 +565,40 @@
         <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>11</v>
+        <v>43</v>
       </c>
       <c r="D2">
         <v>1</v>
       </c>
       <c r="E2" t="s">
-        <v>12</v>
+        <v>45</v>
       </c>
       <c r="F2" t="s">
-        <v>22</v>
+        <v>44</v>
       </c>
       <c r="G2" t="s">
         <v>8</v>
       </c>
       <c r="H2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="I2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="J2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="K2">
         <v>1</v>
       </c>
       <c r="L2" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="M2" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="N2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3">
-        <v>1</v>
-      </c>
-      <c r="E3" t="s">
-        <v>12</v>
-      </c>
-      <c r="F3" t="s">
-        <v>23</v>
-      </c>
-      <c r="G3" t="s">
-        <v>8</v>
-      </c>
-      <c r="H3" t="s">
-        <v>17</v>
-      </c>
-      <c r="I3" t="s">
-        <v>18</v>
-      </c>
-      <c r="J3" t="s">
-        <v>13</v>
-      </c>
-      <c r="K3">
-        <v>2</v>
-      </c>
-      <c r="L3" t="s">
-        <v>37</v>
-      </c>
-      <c r="N3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4">
-        <v>1</v>
-      </c>
-      <c r="E4" t="s">
-        <v>12</v>
-      </c>
-      <c r="F4" t="s">
-        <v>24</v>
-      </c>
-      <c r="G4" t="s">
-        <v>8</v>
-      </c>
-      <c r="H4" t="s">
-        <v>17</v>
-      </c>
-      <c r="I4" t="s">
-        <v>19</v>
-      </c>
-      <c r="J4" t="s">
-        <v>13</v>
-      </c>
-      <c r="K4">
-        <v>3</v>
-      </c>
-      <c r="L4" t="s">
-        <v>37</v>
-      </c>
-      <c r="N4" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D5">
-        <v>1</v>
-      </c>
-      <c r="E5" t="s">
-        <v>12</v>
-      </c>
-      <c r="F5" t="s">
         <v>25</v>
-      </c>
-      <c r="G5" t="s">
-        <v>8</v>
-      </c>
-      <c r="H5" t="s">
-        <v>17</v>
-      </c>
-      <c r="I5" t="s">
-        <v>20</v>
-      </c>
-      <c r="J5" t="s">
-        <v>13</v>
-      </c>
-      <c r="K5">
-        <v>4</v>
-      </c>
-      <c r="L5" t="s">
-        <v>37</v>
-      </c>
-      <c r="N5" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C6" t="s">
-        <v>11</v>
-      </c>
-      <c r="D6">
-        <v>1</v>
-      </c>
-      <c r="E6" t="s">
-        <v>12</v>
-      </c>
-      <c r="F6" t="s">
-        <v>26</v>
-      </c>
-      <c r="G6" t="s">
-        <v>8</v>
-      </c>
-      <c r="H6" t="s">
-        <v>17</v>
-      </c>
-      <c r="I6" t="s">
-        <v>21</v>
-      </c>
-      <c r="J6" t="s">
-        <v>13</v>
-      </c>
-      <c r="K6">
-        <v>2</v>
-      </c>
-      <c r="L6" t="s">
-        <v>37</v>
-      </c>
-      <c r="N6" t="s">
-        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -744,16 +606,197 @@
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" xr:uid="{C3BA60E4-4CD4-4BFC-A771-F46E32D4FCC3}"/>
     <hyperlink ref="B2" r:id="rId2" xr:uid="{885F00E3-8F57-41D1-9044-25B3AFDD29D5}"/>
-    <hyperlink ref="A3" r:id="rId3" xr:uid="{EC0EADC7-2300-4075-866C-D5E6AF7DC158}"/>
-    <hyperlink ref="A4" r:id="rId4" xr:uid="{9621CA98-3790-4FBE-A8AE-4713525BE229}"/>
-    <hyperlink ref="A5" r:id="rId5" xr:uid="{C3A1B03B-250F-4ADC-9E6F-FED719940254}"/>
-    <hyperlink ref="A6" r:id="rId6" xr:uid="{791415A7-1E97-47BB-9E5C-29148A4DB457}"/>
-    <hyperlink ref="B3" r:id="rId7" xr:uid="{E5BF3393-1E8B-408D-9F6F-23D9ED28DD0C}"/>
-    <hyperlink ref="B4" r:id="rId8" xr:uid="{0D3FB2D6-B004-438D-9184-71F9438E9DF8}"/>
-    <hyperlink ref="B5" r:id="rId9" xr:uid="{303F958A-C37C-4ED5-B1E0-97B487262B9F}"/>
-    <hyperlink ref="B6" r:id="rId10" xr:uid="{2F3449FD-5097-481A-859E-BB43EEFA4A33}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId11"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17B4F198-9A04-498F-A15B-0E0D8FA8429A}">
+  <dimension ref="A1:N4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:O4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D1">
+        <v>1</v>
+      </c>
+      <c r="E1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F1" t="s">
+        <v>39</v>
+      </c>
+      <c r="G1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" t="s">
+        <v>15</v>
+      </c>
+      <c r="I1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J1" t="s">
+        <v>11</v>
+      </c>
+      <c r="K1">
+        <v>2</v>
+      </c>
+      <c r="L1" t="s">
+        <v>30</v>
+      </c>
+      <c r="N1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2" t="s">
+        <v>36</v>
+      </c>
+      <c r="F2" t="s">
+        <v>40</v>
+      </c>
+      <c r="G2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J2" t="s">
+        <v>11</v>
+      </c>
+      <c r="K2">
+        <v>3</v>
+      </c>
+      <c r="L2" t="s">
+        <v>30</v>
+      </c>
+      <c r="N2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3" t="s">
+        <v>37</v>
+      </c>
+      <c r="F3" t="s">
+        <v>41</v>
+      </c>
+      <c r="G3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H3" t="s">
+        <v>15</v>
+      </c>
+      <c r="I3" t="s">
+        <v>18</v>
+      </c>
+      <c r="J3" t="s">
+        <v>11</v>
+      </c>
+      <c r="K3">
+        <v>4</v>
+      </c>
+      <c r="L3" t="s">
+        <v>30</v>
+      </c>
+      <c r="N3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4" t="s">
+        <v>38</v>
+      </c>
+      <c r="F4" t="s">
+        <v>42</v>
+      </c>
+      <c r="G4" t="s">
+        <v>8</v>
+      </c>
+      <c r="H4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I4" t="s">
+        <v>19</v>
+      </c>
+      <c r="J4" t="s">
+        <v>11</v>
+      </c>
+      <c r="K4">
+        <v>2</v>
+      </c>
+      <c r="L4" t="s">
+        <v>30</v>
+      </c>
+      <c r="N4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A1" r:id="rId1" xr:uid="{EC0EADC7-2300-4075-866C-D5E6AF7DC158}"/>
+    <hyperlink ref="A2" r:id="rId2" xr:uid="{9621CA98-3790-4FBE-A8AE-4713525BE229}"/>
+    <hyperlink ref="A3" r:id="rId3" xr:uid="{C3A1B03B-250F-4ADC-9E6F-FED719940254}"/>
+    <hyperlink ref="A4" r:id="rId4" xr:uid="{791415A7-1E97-47BB-9E5C-29148A4DB457}"/>
+    <hyperlink ref="B1" r:id="rId5" xr:uid="{E5BF3393-1E8B-408D-9F6F-23D9ED28DD0C}"/>
+    <hyperlink ref="B2" r:id="rId6" xr:uid="{0D3FB2D6-B004-438D-9184-71F9438E9DF8}"/>
+    <hyperlink ref="B3" r:id="rId7" xr:uid="{303F958A-C37C-4ED5-B1E0-97B487262B9F}"/>
+    <hyperlink ref="B4" r:id="rId8" xr:uid="{2F3449FD-5097-481A-859E-BB43EEFA4A33}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>